<commit_message>
Added Password Encryption code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData3.xlsx
+++ b/src/test/resources/testdata/TestData3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974AE50D-E1E8-47CA-B0B8-D804F014C9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254B1AFB-1CFB-458D-ACEB-CB7DAC758223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
     <t>UserRole</t>
   </si>
   <si>
@@ -58,16 +55,19 @@
     <t>Admin1</t>
   </si>
   <si>
-    <t>Login_ValidCredentials</t>
-  </si>
-  <si>
-    <t>Login_InvalidCredentials</t>
-  </si>
-  <si>
-    <t>admin1234</t>
-  </si>
-  <si>
-    <t>SearchUser</t>
+    <t>TC01_Admin_SearchUser</t>
+  </si>
+  <si>
+    <t>TC01_Login_ValidCredentials</t>
+  </si>
+  <si>
+    <t>TC02_Login_InvalidCredentials</t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM0</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -454,10 +454,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>10</v>
@@ -476,13 +476,13 @@
         <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -490,32 +490,32 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>11</v>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,21 +546,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -569,7 +569,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>